<commit_message>
update repository search engine
</commit_message>
<xml_diff>
--- a/buscador/resultados.xlsx
+++ b/buscador/resultados.xlsx
@@ -485,10 +485,10 @@
         <v>80</v>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -497,7 +497,7 @@
         <v>-45</v>
       </c>
       <c r="G2" t="n">
-        <v>131</v>
+        <v>50</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -518,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -527,7 +527,7 @@
         <v>30</v>
       </c>
       <c r="G3" t="n">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -545,10 +545,10 @@
         <v>60</v>
       </c>
       <c r="C4" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D4" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -557,7 +557,7 @@
         <v>-60</v>
       </c>
       <c r="G4" t="n">
-        <v>111</v>
+        <v>45</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -575,10 +575,10 @@
         <v>60</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -587,11 +587,11 @@
         <v>-30</v>
       </c>
       <c r="G5" t="n">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -605,10 +605,10 @@
         <v>80</v>
       </c>
       <c r="C6" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>-20</v>
@@ -617,7 +617,7 @@
         <v>-70</v>
       </c>
       <c r="G6" t="n">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>

</xml_diff>